<commit_message>
modified:   BattleField/BattleField.py 	modified:   "Document/50kg\345\260\217\351\243\236\346\234\272\345\220\216\347\273\255.xlsx" 	modified:   MissionGym/Gym_test.py 	modified:   MissionGym/UAV_Patrol_gym/envs/UAV_Patrol_env.py 	"Document/~$50kg\345\260\217\351\243\236\346\234\272\345\220\216\347\273\255.xlsx" 	"Document/\344\270\213\344\270\200\350\275\256\351\227\256\351\242\2302023\345\271\2646\346\234\21013\346\227\245\345\273\272\345\210\266.txt"
</commit_message>
<xml_diff>
--- a/Document/50kg小飞机后续.xlsx
+++ b/Document/50kg小飞机后续.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>智能无人机任务规划这个方面去做。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -402,6 +402,22 @@
   </si>
   <si>
     <t>但是貌似还可以聊，要是小于三公里，那真就聊不了了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月13日19:56:43终于避无可避了，要好好动脑子想想，那个矩阵要怎么给出了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首先一个问题，是把目标的矩阵还是把某种扫过的矩阵作为evaluate array？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>而目标的那个只含有某种固定的“边界”性质的东西。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扫过的就相当于含有所有历史信息了。先采用这个，无人机知道自己飞过了什么地方，不是理所当然的吗。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1020,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:V80"/>
+  <dimension ref="B7:V87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1490,6 +1506,26 @@
         <v>96</v>
       </c>
     </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
modified:   BattleField/BattleField.py 	new file:   BattleField/BattleField2.py 	new file:   BattleField/shishiThreadPool.py 	modified:   BattleField/void/shishi.png 	modified:   "Document/50kg\345\260\217\351\243\236\346\234\272\345\220\216\347\273\255.xlsx" 	new file:   "Document/\344\270\213\344\270\200\350\275\256\351\227\256\351\242\2302023\345\271\2646\346\234\21013\346\227\245\345\273\272\345\210\266.txt" 	modified:   MissionGym/Gym_test.py 	modified:   MissionGym/UAV_Patrol_gym/envs/UAV_Patrol_env.py 	modified:   UAV/__pycache__/UAV.cpython-35.pyc
</commit_message>
<xml_diff>
--- a/Document/50kg小飞机后续.xlsx
+++ b/Document/50kg小飞机后续.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
     <t>智能无人机任务规划这个方面去做。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -418,6 +418,173 @@
   </si>
   <si>
     <t>扫过的就相当于含有所有历史信息了。先采用这个，无人机知道自己飞过了什么地方，不是理所当然的吗。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个很关键的参数就是刷新率，或者说轨道周期，总之就是过一次能用上的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月14日11:28:25测了一下运行速度，运行速度有点慢呀，是不是矩阵太多了。还是判断距离的那部分太多了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200秒算了一千步，说慢也不算慢，但是肯定也算不上快就是了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恐怕真的得琢磨一下什么线程池机制啊之类的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU占用并不高，说明是单核的。如果开个8核就可以变成几十秒一步了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那么问题就来了，是多线程还是改矩阵呢？反正分析下来最大的时间消耗还是在node更新状态这一步。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看起来还是线程池比较好改，对程序的改动比较小。改矩阵会损失可读性。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好，决定了，就改线程池。刚好相当于CPU和GPU都用起来了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2秒一步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多线程改起来挺快的，但是线程是开起来了，CPU占用并没有上去。这就尴尬了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好吧，好像小有增加，但显然没有拉满。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线程数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000步耗时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月14日14:36:37生成几何还是有问题，现在这个检测不出那种不连续的点凹进去的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看来得整一个偏转角度检测，超过360度直接寄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好像没什么变化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好像还是没什么变化。这相当于是计算密集型的东西了，搞来搞去都是它自己Python解释器在算，不像之前可以调用外面的东西，所以效果没什么变化？是这个道理吗。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那意思还得攒一个C++的计算库进来？用于给你并行？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/595502483，行吧，真有人这么干来实现多线程的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/383572973，这个，好像靠谱。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行吧，那就整一下。想必不会比JNI更加蛋疼吧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月14日17:21:13，实现了demo，但是改写起来恐怕挺蛋疼的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草了，有那么一瞬间甚至在怀疑，用Python写是不是错误的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那传参数这部分还挺麻烦的呀，至少传一个list进去肯定是跑不了的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pybind11.readthedocs.io/en/stable/advanced/pycpp/object.html</t>
+  </si>
+  <si>
+    <t>文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不行，只能传基础的参数类型，不能传自定义的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把求距离的部分并行出去，别的仍然放在Python这头，应该是比较好的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算是把C++的弄进去了，看一下效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线程数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000步耗时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU占比确实是增加了一些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算是稍微有点效果。进一步封装一下估计还能更好点儿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和3的相比，CPU占比并没有显著的增加，说明还是寄？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好，这次是把判断也挪进去了，这样不用往node里面传UAV了，C++传回来的也直接是bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>什么东西？CPU占用反而是降低了？是因为删了time，sleep？2023年6月15日14:35:57好像是，加上之后貌似恢复了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算是稍微又有一点点效果，但是显然没有实现把CPU拉满的目标。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月15日14:44:02，艹，实在不行就直接C++写一个battlefiled？现在至少是掌握了可能性的。要不就是改成矩阵版本的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>要不就是进一步改进算法，node用范围定义，然后只更新周围的点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总之就是也差不多，没什么前途。还得是好好优化算法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月15日16:53:52好，程序大改完事儿了。避免了大量的不必要的重复计算，代价是程序可读性下降和复杂性增加。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好这下好了，变成6秒了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1036,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:V87"/>
+  <dimension ref="B7:V122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1506,24 +1673,270 @@
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:19" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="Q85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="3:19" x14ac:dyDescent="0.2">
       <c r="E86" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:19" x14ac:dyDescent="0.2">
       <c r="E87" t="s">
         <v>99</v>
+      </c>
+      <c r="R87" t="s">
+        <v>103</v>
+      </c>
+      <c r="S87" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="R88" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>101</v>
+      </c>
+      <c r="R89" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="Q91" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>114</v>
+      </c>
+      <c r="R92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>115</v>
+      </c>
+      <c r="R93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="Q95" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="R96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>112</v>
+      </c>
+      <c r="R97" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q98">
+        <v>3</v>
+      </c>
+      <c r="R98">
+        <v>205</v>
+      </c>
+      <c r="T98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q99">
+        <v>6</v>
+      </c>
+      <c r="T99" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q102" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q103" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="105" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>6.2612535953521702</v>
+      </c>
+      <c r="E105">
+        <v>6.2253460884094203</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="R106" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <f>R115/D105</f>
+        <v>30.370025879229477</v>
+      </c>
+    </row>
+    <row r="108" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q108" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q109" t="s">
+        <v>126</v>
+      </c>
+      <c r="R109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="Q110" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="R111" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q113" t="s">
+        <v>129</v>
+      </c>
+      <c r="U113" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q114" t="s">
+        <v>130</v>
+      </c>
+      <c r="R114" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="115" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q115">
+        <v>3</v>
+      </c>
+      <c r="R115">
+        <v>190.15443372726401</v>
+      </c>
+      <c r="S115">
+        <v>182.33571934700001</v>
+      </c>
+      <c r="V115" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q116">
+        <v>6</v>
+      </c>
+      <c r="R116">
+        <v>179.96466469764701</v>
+      </c>
+      <c r="S116">
+        <v>182.988606929779</v>
+      </c>
+      <c r="T116">
+        <v>179.21554517745901</v>
+      </c>
+      <c r="V116" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q119" t="s">
+        <v>135</v>
+      </c>
+      <c r="U119" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="120" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q120" t="s">
+        <v>130</v>
+      </c>
+      <c r="R120" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q121">
+        <v>3</v>
+      </c>
+      <c r="R121">
+        <f>175.22634601593</f>
+        <v>175.22634601593001</v>
+      </c>
+      <c r="S121">
+        <v>175.24729108810399</v>
+      </c>
+      <c r="V121" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q122">
+        <v>6</v>
+      </c>
+      <c r="R122">
+        <v>175.37919330596901</v>
+      </c>
+      <c r="V122" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1531,8 +1944,11 @@
   <hyperlinks>
     <hyperlink ref="D34" r:id="rId1"/>
     <hyperlink ref="D35" r:id="rId2"/>
+    <hyperlink ref="Q102" r:id="rId3"/>
+    <hyperlink ref="Q103" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   Agent/actor_network.py 	new file:   Agent/critic_network.py 	new file:   Agent/replay_buffer.py 	modified:   "Document/50kg\345\260\217\351\243\236\346\234\272\345\220\216\347\273\255.xlsx"
</commit_message>
<xml_diff>
--- a/Document/50kg小飞机后续.xlsx
+++ b/Document/50kg小飞机后续.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
   <si>
     <t>智能无人机任务规划这个方面去做。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -585,6 +585,26 @@
   </si>
   <si>
     <t>好这下好了，变成6秒了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月16日09:53:45继续，赶紧开始整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看了CNN的示例代码。感觉不是很复杂呀。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年6月16日16:41:03讲道理，不要跳步骤，先搞到倒立摆能够摆起来，再考虑别的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还是得要transfer，尽量把能映射的都映射成0-1或者-1,1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现已明确，强化学习就是会过分拟合的，当年的某个面试的人就是个傻逼东西。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1135,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R55"/>
+  <dimension ref="B2:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1173,24 +1193,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1205,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:V122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>